<commit_message>
Updated WECC 179 bus system with info.
</commit_message>
<xml_diff>
--- a/andes/cases/wecc/wecc179.xlsx
+++ b/andes/cases/wecc/wecc179.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hcui7/repos/andes/andes/cases/wecc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41808DB7-7CA6-BF42-BEF1-EA700829EACE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{844BAD5A-DEC3-7E49-B8B7-714C23A4C7F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="4060" windowWidth="18660" windowHeight="14500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3200" yWindow="4200" windowWidth="25040" windowHeight="18900" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -21,13 +21,14 @@
     <sheet name="Line" sheetId="6" r:id="rId6"/>
     <sheet name="GENCLS" sheetId="7" r:id="rId7"/>
     <sheet name="Toggler" sheetId="8" r:id="rId8"/>
+    <sheet name="Fault" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="650">
   <si>
     <t>idx</t>
   </si>
@@ -539,9 +540,6 @@
     <t>q0</t>
   </si>
   <si>
-    <t>PQ_0</t>
-  </si>
-  <si>
     <t>PQ_1</t>
   </si>
   <si>
@@ -851,6 +849,9 @@
     <t>PQ_103</t>
   </si>
   <si>
+    <t>PQ_104</t>
+  </si>
+  <si>
     <t>Sn</t>
   </si>
   <si>
@@ -884,9 +885,6 @@
     <t>fn</t>
   </si>
   <si>
-    <t>Shunt_0</t>
-  </si>
-  <si>
     <t>Shunt_1</t>
   </si>
   <si>
@@ -1004,6 +1002,9 @@
     <t>Shunt_39</t>
   </si>
   <si>
+    <t>Shunt_40</t>
+  </si>
+  <si>
     <t>bus1</t>
   </si>
   <si>
@@ -1043,9 +1044,6 @@
     <t>phi</t>
   </si>
   <si>
-    <t>Line_0</t>
-  </si>
-  <si>
     <t>Line_1</t>
   </si>
   <si>
@@ -1832,6 +1830,9 @@
     <t>Line_262</t>
   </si>
   <si>
+    <t>Line_263</t>
+  </si>
+  <si>
     <t>gen</t>
   </si>
   <si>
@@ -1862,9 +1863,6 @@
     <t>S12</t>
   </si>
   <si>
-    <t>GENCLS_0</t>
-  </si>
-  <si>
     <t>GENCLS_1</t>
   </si>
   <si>
@@ -1949,6 +1947,9 @@
     <t>GENCLS_28</t>
   </si>
   <si>
+    <t>GENCLS_29</t>
+  </si>
+  <si>
     <t>model</t>
   </si>
   <si>
@@ -1962,6 +1963,21 @@
   </si>
   <si>
     <t>Line</t>
+  </si>
+  <si>
+    <t>tf</t>
+  </si>
+  <si>
+    <t>tc</t>
+  </si>
+  <si>
+    <t>xf</t>
+  </si>
+  <si>
+    <t>rf</t>
+  </si>
+  <si>
+    <t>Fault_1</t>
   </si>
 </sst>
 </file>
@@ -2367,7 +2383,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K13" sqref="K13"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10301,7 +10317,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -10369,10 +10385,10 @@
         <v>-0.56000000000000005</v>
       </c>
       <c r="I2">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J2">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K2">
         <v>1</v>
@@ -10404,10 +10420,10 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J3">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K3">
         <v>1</v>
@@ -10439,10 +10455,10 @@
         <v>-1.27</v>
       </c>
       <c r="I4">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J4">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -10474,10 +10490,10 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J5">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K5">
         <v>1</v>
@@ -10509,10 +10525,10 @@
         <v>-0.56000000000000005</v>
       </c>
       <c r="I6">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J6">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K6">
         <v>1</v>
@@ -10544,10 +10560,10 @@
         <v>0</v>
       </c>
       <c r="I7">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J7">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K7">
         <v>1</v>
@@ -10579,10 +10595,10 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="I8">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J8">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K8">
         <v>1</v>
@@ -10614,10 +10630,10 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J9">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K9">
         <v>1</v>
@@ -10649,10 +10665,10 @@
         <v>0.7</v>
       </c>
       <c r="I10">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J10">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K10">
         <v>1</v>
@@ -10684,10 +10700,10 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J11">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K11">
         <v>1</v>
@@ -10719,10 +10735,10 @@
         <v>0</v>
       </c>
       <c r="I12">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J12">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K12">
         <v>1</v>
@@ -10754,10 +10770,10 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="I13">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J13">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K13">
         <v>1</v>
@@ -10789,10 +10805,10 @@
         <v>0.05</v>
       </c>
       <c r="I14">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J14">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K14">
         <v>1</v>
@@ -10824,10 +10840,10 @@
         <v>0</v>
       </c>
       <c r="I15">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J15">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K15">
         <v>1</v>
@@ -10859,10 +10875,10 @@
         <v>-0.69</v>
       </c>
       <c r="I16">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J16">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K16">
         <v>1</v>
@@ -10894,10 +10910,10 @@
         <v>0</v>
       </c>
       <c r="I17">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J17">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K17">
         <v>1</v>
@@ -10929,10 +10945,10 @@
         <v>10</v>
       </c>
       <c r="I18">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J18">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K18">
         <v>1</v>
@@ -10964,10 +10980,10 @@
         <v>7</v>
       </c>
       <c r="I19">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J19">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K19">
         <v>1</v>
@@ -10999,10 +11015,10 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J20">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K20">
         <v>1</v>
@@ -11034,10 +11050,10 @@
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J21">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K21">
         <v>1</v>
@@ -11069,10 +11085,10 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="I22">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J22">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K22">
         <v>1</v>
@@ -11104,10 +11120,10 @@
         <v>0</v>
       </c>
       <c r="I23">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J23">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K23">
         <v>1</v>
@@ -11139,10 +11155,10 @@
         <v>0.27</v>
       </c>
       <c r="I24">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J24">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -11174,10 +11190,10 @@
         <v>0</v>
       </c>
       <c r="I25">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J25">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K25">
         <v>1</v>
@@ -11209,10 +11225,10 @@
         <v>9.0709999999999997</v>
       </c>
       <c r="I26">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J26">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K26">
         <v>1</v>
@@ -11244,10 +11260,10 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J27">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K27">
         <v>1</v>
@@ -11279,10 +11295,10 @@
         <v>-0.17</v>
       </c>
       <c r="I28">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J28">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K28">
         <v>1</v>
@@ -11314,10 +11330,10 @@
         <v>0</v>
       </c>
       <c r="I29">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J29">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -11349,10 +11365,10 @@
         <v>0.25</v>
       </c>
       <c r="I30">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J30">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K30">
         <v>1</v>
@@ -11384,10 +11400,10 @@
         <v>0.65</v>
       </c>
       <c r="I31">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J31">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K31">
         <v>1</v>
@@ -11419,10 +11435,10 @@
         <v>-0.63200000000000001</v>
       </c>
       <c r="I32">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J32">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -11454,10 +11470,10 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="I33">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J33">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K33">
         <v>1</v>
@@ -11489,10 +11505,10 @@
         <v>1.321</v>
       </c>
       <c r="I34">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J34">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K34">
         <v>1</v>
@@ -11524,10 +11540,10 @@
         <v>0.24</v>
       </c>
       <c r="I35">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J35">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K35">
         <v>1</v>
@@ -11559,10 +11575,10 @@
         <v>0.25</v>
       </c>
       <c r="I36">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J36">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K36">
         <v>1</v>
@@ -11594,10 +11610,10 @@
         <v>-6.2E-2</v>
       </c>
       <c r="I37">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J37">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K37">
         <v>1</v>
@@ -11629,10 +11645,10 @@
         <v>16.54</v>
       </c>
       <c r="I38">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J38">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K38">
         <v>1</v>
@@ -11664,10 +11680,10 @@
         <v>0.80599999999999994</v>
       </c>
       <c r="I39">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J39">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K39">
         <v>1</v>
@@ -11699,10 +11715,10 @@
         <v>0.17599999999999999</v>
       </c>
       <c r="I40">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J40">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K40">
         <v>1</v>
@@ -11734,10 +11750,10 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="I41">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J41">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K41">
         <v>1</v>
@@ -11769,10 +11785,10 @@
         <v>0</v>
       </c>
       <c r="I42">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J42">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K42">
         <v>1</v>
@@ -11804,10 +11820,10 @@
         <v>3</v>
       </c>
       <c r="I43">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J43">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K43">
         <v>1</v>
@@ -11839,10 +11855,10 @@
         <v>0.3125</v>
       </c>
       <c r="I44">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J44">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K44">
         <v>1</v>
@@ -11874,10 +11890,10 @@
         <v>1.6</v>
       </c>
       <c r="I45">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J45">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K45">
         <v>1</v>
@@ -11909,10 +11925,10 @@
         <v>0.22</v>
       </c>
       <c r="I46">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J46">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K46">
         <v>1</v>
@@ -11944,10 +11960,10 @@
         <v>0</v>
       </c>
       <c r="I47">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J47">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K47">
         <v>1</v>
@@ -11979,10 +11995,10 @@
         <v>16.809999999999999</v>
       </c>
       <c r="I48">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J48">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K48">
         <v>1</v>
@@ -12014,10 +12030,10 @@
         <v>-0.5</v>
       </c>
       <c r="I49">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J49">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K49">
         <v>1</v>
@@ -12049,10 +12065,10 @@
         <v>3.94</v>
       </c>
       <c r="I50">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J50">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K50">
         <v>1</v>
@@ -12084,10 +12100,10 @@
         <v>11</v>
       </c>
       <c r="I51">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J51">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K51">
         <v>1</v>
@@ -12119,10 +12135,10 @@
         <v>0</v>
       </c>
       <c r="I52">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J52">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K52">
         <v>1</v>
@@ -12154,10 +12170,10 @@
         <v>5</v>
       </c>
       <c r="I53">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J53">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K53">
         <v>1</v>
@@ -12189,10 +12205,10 @@
         <v>0</v>
       </c>
       <c r="I54">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J54">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K54">
         <v>1</v>
@@ -12224,10 +12240,10 @@
         <v>4</v>
       </c>
       <c r="I55">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J55">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K55">
         <v>1</v>
@@ -12259,10 +12275,10 @@
         <v>-0.97</v>
       </c>
       <c r="I56">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J56">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K56">
         <v>1</v>
@@ -12294,10 +12310,10 @@
         <v>-1.19</v>
       </c>
       <c r="I57">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J57">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K57">
         <v>1</v>
@@ -12329,10 +12345,10 @@
         <v>-4.1399999999999997</v>
       </c>
       <c r="I58">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J58">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K58">
         <v>1</v>
@@ -12364,10 +12380,10 @@
         <v>0.2</v>
       </c>
       <c r="I59">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J59">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K59">
         <v>1</v>
@@ -12399,10 +12415,10 @@
         <v>-0.77</v>
       </c>
       <c r="I60">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J60">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K60">
         <v>1</v>
@@ -12434,10 +12450,10 @@
         <v>0.25</v>
       </c>
       <c r="I61">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J61">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K61">
         <v>1</v>
@@ -12469,10 +12485,10 @@
         <v>0</v>
       </c>
       <c r="I62">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J62">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K62">
         <v>1</v>
@@ -12504,10 +12520,10 @@
         <v>-7.5999999999999998E-2</v>
       </c>
       <c r="I63">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J63">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K63">
         <v>1</v>
@@ -12539,10 +12555,10 @@
         <v>-1E-3</v>
       </c>
       <c r="I64">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J64">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K64">
         <v>1</v>
@@ -12574,10 +12590,10 @@
         <v>0</v>
       </c>
       <c r="I65">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J65">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K65">
         <v>1</v>
@@ -12609,10 +12625,10 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="I66">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J66">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K66">
         <v>1</v>
@@ -12644,10 +12660,10 @@
         <v>-3.29</v>
       </c>
       <c r="I67">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J67">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K67">
         <v>1</v>
@@ -12679,10 +12695,10 @@
         <v>0.32600000000000001</v>
       </c>
       <c r="I68">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J68">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K68">
         <v>1</v>
@@ -12714,10 +12730,10 @@
         <v>0.215</v>
       </c>
       <c r="I69">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J69">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K69">
         <v>1</v>
@@ -12749,10 +12765,10 @@
         <v>0.61499999999999999</v>
       </c>
       <c r="I70">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J70">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K70">
         <v>1</v>
@@ -12784,10 +12800,10 @@
         <v>0</v>
       </c>
       <c r="I71">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J71">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K71">
         <v>1</v>
@@ -12819,10 +12835,10 @@
         <v>0</v>
       </c>
       <c r="I72">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J72">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K72">
         <v>1</v>
@@ -12854,10 +12870,10 @@
         <v>1.1850000000000001</v>
       </c>
       <c r="I73">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J73">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K73">
         <v>1</v>
@@ -12889,10 +12905,10 @@
         <v>0</v>
       </c>
       <c r="I74">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J74">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K74">
         <v>1</v>
@@ -12924,10 +12940,10 @@
         <v>0.54799999999999993</v>
       </c>
       <c r="I75">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J75">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K75">
         <v>1</v>
@@ -12959,10 +12975,10 @@
         <v>0</v>
       </c>
       <c r="I76">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J76">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K76">
         <v>1</v>
@@ -12994,10 +13010,10 @@
         <v>34.909999999999997</v>
       </c>
       <c r="I77">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J77">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K77">
         <v>1</v>
@@ -13029,10 +13045,10 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="I78">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J78">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K78">
         <v>1</v>
@@ -13064,10 +13080,10 @@
         <v>0.18</v>
       </c>
       <c r="I79">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J79">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K79">
         <v>1</v>
@@ -13099,10 +13115,10 @@
         <v>0</v>
       </c>
       <c r="I80">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J80">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K80">
         <v>1</v>
@@ -13134,10 +13150,10 @@
         <v>-0.114</v>
       </c>
       <c r="I81">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J81">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K81">
         <v>1</v>
@@ -13169,10 +13185,10 @@
         <v>0</v>
       </c>
       <c r="I82">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J82">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K82">
         <v>1</v>
@@ -13204,10 +13220,10 @@
         <v>6.3</v>
       </c>
       <c r="I83">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J83">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K83">
         <v>1</v>
@@ -13239,10 +13255,10 @@
         <v>-0.28199999999999997</v>
       </c>
       <c r="I84">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J84">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K84">
         <v>1</v>
@@ -13274,10 +13290,10 @@
         <v>0.64500000000000002</v>
       </c>
       <c r="I85">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J85">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K85">
         <v>1</v>
@@ -13309,10 +13325,10 @@
         <v>0</v>
       </c>
       <c r="I86">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J86">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K86">
         <v>1</v>
@@ -13344,10 +13360,10 @@
         <v>11.89</v>
       </c>
       <c r="I87">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J87">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K87">
         <v>1</v>
@@ -13379,10 +13395,10 @@
         <v>0</v>
       </c>
       <c r="I88">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J88">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K88">
         <v>1</v>
@@ -13414,10 +13430,10 @@
         <v>0</v>
       </c>
       <c r="I89">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J89">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K89">
         <v>1</v>
@@ -13449,10 +13465,10 @@
         <v>0.78</v>
       </c>
       <c r="I90">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J90">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K90">
         <v>1</v>
@@ -13484,10 +13500,10 @@
         <v>0.72799999999999998</v>
       </c>
       <c r="I91">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J91">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K91">
         <v>1</v>
@@ -13519,10 +13535,10 @@
         <v>0.41</v>
       </c>
       <c r="I92">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J92">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K92">
         <v>1</v>
@@ -13554,10 +13570,10 @@
         <v>-0.108</v>
       </c>
       <c r="I93">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J93">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K93">
         <v>1</v>
@@ -13589,10 +13605,10 @@
         <v>0.81700000000000006</v>
       </c>
       <c r="I94">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J94">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K94">
         <v>1</v>
@@ -13624,10 +13640,10 @@
         <v>0.11899999999999999</v>
       </c>
       <c r="I95">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J95">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K95">
         <v>1</v>
@@ -13659,10 +13675,10 @@
         <v>-7.9000000000000001E-2</v>
       </c>
       <c r="I96">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J96">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K96">
         <v>1</v>
@@ -13694,10 +13710,10 @@
         <v>0.38400000000000001</v>
       </c>
       <c r="I97">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J97">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K97">
         <v>1</v>
@@ -13729,10 +13745,10 @@
         <v>0</v>
       </c>
       <c r="I98">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J98">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K98">
         <v>1</v>
@@ -13764,10 +13780,10 @@
         <v>0.128</v>
       </c>
       <c r="I99">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J99">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K99">
         <v>1</v>
@@ -13799,10 +13815,10 @@
         <v>1</v>
       </c>
       <c r="I100">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J100">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K100">
         <v>1</v>
@@ -13834,10 +13850,10 @@
         <v>0</v>
       </c>
       <c r="I101">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J101">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K101">
         <v>1</v>
@@ -13869,10 +13885,10 @@
         <v>0.115</v>
       </c>
       <c r="I102">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J102">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K102">
         <v>1</v>
@@ -13904,10 +13920,10 @@
         <v>0.71400000000000008</v>
       </c>
       <c r="I103">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J103">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K103">
         <v>1</v>
@@ -13939,10 +13955,10 @@
         <v>-0.43</v>
       </c>
       <c r="I104">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J104">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K104">
         <v>1</v>
@@ -13974,10 +13990,10 @@
         <v>0.78500000000000003</v>
       </c>
       <c r="I105">
-        <v>1.25</v>
+        <v>1.2</v>
       </c>
       <c r="J105">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="K105">
         <v>1</v>
@@ -17101,8 +17117,8 @@
   <dimension ref="A1:X264"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -35981,12 +35997,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9FCFDCF-0C65-464C-A0A5-095984B80698}">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -36015,11 +36031,11 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>643</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -36035,6 +36051,80 @@
       </c>
       <c r="G2">
         <v>1.1000000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28D773FF-68DA-644D-863B-34214F4BF4E4}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>646</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>647</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>649</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>649</v>
+      </c>
+      <c r="E2">
+        <v>85</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H2">
+        <v>1E-3</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>